<commit_message>
chapter 3 -4 update
</commit_message>
<xml_diff>
--- a/0_MARCH_3_2022/POF_Documentation/Expences.xlsx
+++ b/0_MARCH_3_2022/POF_Documentation/Expences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Makoy files_DONT REMOVE\Computer-Engineering-Practice-and-Design-2\0_MARCH_3_2022\POF_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960811EA-0F90-498A-A7E2-A633191297DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382338CC-5FEA-40A1-B767-E336F508FE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34E937BC-3B4F-43D1-B580-D634078245D1}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>fare sa van</t>
+  </si>
+  <si>
+    <t>UVC LAMP</t>
+  </si>
+  <si>
+    <t>petri dish</t>
+  </si>
+  <si>
+    <t>premixed nutrient agar</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AC3C42-CD89-4EF1-9A03-CFA0B70CDF56}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -715,6 +724,33 @@
         <v>6</v>
       </c>
     </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1700</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44774</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>202</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>257</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>